<commit_message>
initial version of stimuli order
</commit_message>
<xml_diff>
--- a/sequences/00_cues.xlsx
+++ b/sequences/00_cues.xlsx
@@ -25,196 +25,196 @@
     <t>category</t>
   </si>
   <si>
-    <t>face/face124.png</t>
+    <t>face/face097.png</t>
+  </si>
+  <si>
+    <t>car/car113.png</t>
+  </si>
+  <si>
+    <t>face/face096.png</t>
+  </si>
+  <si>
+    <t>face/face073.png</t>
+  </si>
+  <si>
+    <t>face/face072.png</t>
+  </si>
+  <si>
+    <t>car/car109.png</t>
+  </si>
+  <si>
+    <t>face/face091.png</t>
+  </si>
+  <si>
+    <t>car/car066.png</t>
+  </si>
+  <si>
+    <t>car/car067.png</t>
+  </si>
+  <si>
+    <t>car/car121.png</t>
+  </si>
+  <si>
+    <t>car/car081.png</t>
+  </si>
+  <si>
+    <t>car/car082.png</t>
+  </si>
+  <si>
+    <t>face/face108.png</t>
+  </si>
+  <si>
+    <t>car/car102.png</t>
+  </si>
+  <si>
+    <t>face/face090.png</t>
+  </si>
+  <si>
+    <t>face/face080.png</t>
+  </si>
+  <si>
+    <t>face/face071.png</t>
+  </si>
+  <si>
+    <t>car/car071.png</t>
+  </si>
+  <si>
+    <t>car/car080.png</t>
+  </si>
+  <si>
+    <t>car/car089.png</t>
+  </si>
+  <si>
+    <t>face/face065.png</t>
+  </si>
+  <si>
+    <t>face/face092.png</t>
+  </si>
+  <si>
+    <t>face/face121.png</t>
   </si>
   <si>
     <t>face/face103.png</t>
   </si>
   <si>
+    <t>face/face085.png</t>
+  </si>
+  <si>
     <t>car/car111.png</t>
   </si>
   <si>
-    <t>face/face092.png</t>
-  </si>
-  <si>
-    <t>face/face100.png</t>
-  </si>
-  <si>
-    <t>car/car081.png</t>
-  </si>
-  <si>
-    <t>car/car093.png</t>
-  </si>
-  <si>
-    <t>car/car083.png</t>
-  </si>
-  <si>
-    <t>face/face091.png</t>
-  </si>
-  <si>
-    <t>car/car066.png</t>
-  </si>
-  <si>
-    <t>face/face064.png</t>
-  </si>
-  <si>
-    <t>car/car082.png</t>
-  </si>
-  <si>
-    <t>car/car087.png</t>
-  </si>
-  <si>
-    <t>face/face109.png</t>
-  </si>
-  <si>
-    <t>car/car099.png</t>
-  </si>
-  <si>
-    <t>face/face081.png</t>
-  </si>
-  <si>
-    <t>car/car070.png</t>
-  </si>
-  <si>
-    <t>car/car067.png</t>
-  </si>
-  <si>
-    <t>face/face074.png</t>
-  </si>
-  <si>
-    <t>face/face106.png</t>
-  </si>
-  <si>
-    <t>car/car095.png</t>
-  </si>
-  <si>
-    <t>face/face075.png</t>
-  </si>
-  <si>
-    <t>car/car080.png</t>
-  </si>
-  <si>
-    <t>car/car079.png</t>
-  </si>
-  <si>
-    <t>car/car064.png</t>
-  </si>
-  <si>
-    <t>car/car091.png</t>
-  </si>
-  <si>
-    <t>face/face094.png</t>
-  </si>
-  <si>
-    <t>face/face095.png</t>
-  </si>
-  <si>
-    <t>car/car075.png</t>
-  </si>
-  <si>
-    <t>face/face068.png</t>
-  </si>
-  <si>
-    <t>face/face097.png</t>
-  </si>
-  <si>
-    <t>face/face096.png</t>
+    <t>car/car112.png</t>
+  </si>
+  <si>
+    <t>car/car069.png</t>
+  </si>
+  <si>
+    <t>car/car116.png</t>
+  </si>
+  <si>
+    <t>face/face086.png</t>
+  </si>
+  <si>
+    <t>car/car077.png</t>
+  </si>
+  <si>
+    <t>face/face123.png</t>
+  </si>
+  <si>
+    <t>atmen</t>
+  </si>
+  <si>
+    <t>nullen</t>
+  </si>
+  <si>
+    <t>deuten</t>
+  </si>
+  <si>
+    <t>süßen</t>
+  </si>
+  <si>
+    <t>reisen</t>
+  </si>
+  <si>
+    <t>sparen</t>
+  </si>
+  <si>
+    <t>hacken</t>
+  </si>
+  <si>
+    <t>legen</t>
+  </si>
+  <si>
+    <t>wehen</t>
+  </si>
+  <si>
+    <t>frischen</t>
   </si>
   <si>
     <t>danken</t>
   </si>
   <si>
-    <t>ärgern</t>
-  </si>
-  <si>
-    <t>kürzen</t>
-  </si>
-  <si>
-    <t>strahlen</t>
-  </si>
-  <si>
-    <t>feiern</t>
-  </si>
-  <si>
-    <t>sinken</t>
-  </si>
-  <si>
-    <t>hexen</t>
-  </si>
-  <si>
-    <t>boxen</t>
-  </si>
-  <si>
-    <t>stärken</t>
-  </si>
-  <si>
-    <t>segeln</t>
-  </si>
-  <si>
-    <t>lesen</t>
-  </si>
-  <si>
-    <t>drohen</t>
-  </si>
-  <si>
-    <t>handeln</t>
-  </si>
-  <si>
-    <t>sieben</t>
-  </si>
-  <si>
-    <t>lauten</t>
-  </si>
-  <si>
-    <t>räumen</t>
-  </si>
-  <si>
-    <t>süßen</t>
-  </si>
-  <si>
-    <t>proben</t>
-  </si>
-  <si>
-    <t>schmecken</t>
-  </si>
-  <si>
-    <t>bremsen</t>
-  </si>
-  <si>
-    <t>putzen</t>
-  </si>
-  <si>
-    <t>fesseln</t>
-  </si>
-  <si>
-    <t>trotzen</t>
-  </si>
-  <si>
-    <t>ahnen</t>
+    <t>passen</t>
+  </si>
+  <si>
+    <t>küssen</t>
+  </si>
+  <si>
+    <t>meinen</t>
+  </si>
+  <si>
+    <t>ändern</t>
+  </si>
+  <si>
+    <t>öffnen</t>
+  </si>
+  <si>
+    <t>wählen</t>
   </si>
   <si>
     <t>wecken</t>
   </si>
   <si>
-    <t>baden</t>
-  </si>
-  <si>
-    <t>gnaden</t>
-  </si>
-  <si>
-    <t>tanzen</t>
-  </si>
-  <si>
-    <t>rühren</t>
-  </si>
-  <si>
-    <t>sondern</t>
-  </si>
-  <si>
-    <t>heulen</t>
-  </si>
-  <si>
-    <t>münzen</t>
+    <t>leeren</t>
+  </si>
+  <si>
+    <t>tollen</t>
+  </si>
+  <si>
+    <t>rechnen</t>
+  </si>
+  <si>
+    <t>zögern</t>
+  </si>
+  <si>
+    <t>bergen</t>
+  </si>
+  <si>
+    <t>dienen</t>
+  </si>
+  <si>
+    <t>planen</t>
+  </si>
+  <si>
+    <t>herrschen</t>
+  </si>
+  <si>
+    <t>stoßen</t>
+  </si>
+  <si>
+    <t>piepen</t>
+  </si>
+  <si>
+    <t>hassen</t>
+  </si>
+  <si>
+    <t>duschen</t>
+  </si>
+  <si>
+    <t>fließen</t>
+  </si>
+  <si>
+    <t>streifen</t>
   </si>
   <si>
     <t>face</t>
@@ -620,7 +620,7 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -690,7 +690,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -718,7 +718,7 @@
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -746,7 +746,7 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -774,7 +774,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -788,7 +788,7 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -802,7 +802,7 @@
         <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -830,7 +830,7 @@
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -858,7 +858,7 @@
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -872,7 +872,7 @@
         <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -886,7 +886,7 @@
         <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -914,7 +914,7 @@
         <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -928,7 +928,7 @@
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -942,7 +942,7 @@
         <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -970,7 +970,7 @@
         <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -984,7 +984,7 @@
         <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1026,7 +1026,7 @@
         <v>65</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4">

</xml_diff>

<commit_message>
Newest version of experiment
</commit_message>
<xml_diff>
--- a/sequences/00_cues.xlsx
+++ b/sequences/00_cues.xlsx
@@ -25,202 +25,202 @@
     <t>category</t>
   </si>
   <si>
+    <t>face/face070.png</t>
+  </si>
+  <si>
+    <t>house/house095.png</t>
+  </si>
+  <si>
+    <t>house/house075.png</t>
+  </si>
+  <si>
+    <t>face/face069.png</t>
+  </si>
+  <si>
+    <t>face/face108.png</t>
+  </si>
+  <si>
+    <t>house/house125.png</t>
+  </si>
+  <si>
+    <t>face/face092.png</t>
+  </si>
+  <si>
+    <t>house/house117.png</t>
+  </si>
+  <si>
+    <t>face/face099.png</t>
+  </si>
+  <si>
+    <t>house/house091.png</t>
+  </si>
+  <si>
+    <t>face/face094.png</t>
+  </si>
+  <si>
+    <t>house/house094.png</t>
+  </si>
+  <si>
+    <t>face/face064.png</t>
+  </si>
+  <si>
+    <t>face/face096.png</t>
+  </si>
+  <si>
+    <t>face/face101.png</t>
+  </si>
+  <si>
+    <t>house/house082.png</t>
+  </si>
+  <si>
+    <t>house/house086.png</t>
+  </si>
+  <si>
+    <t>face/face090.png</t>
+  </si>
+  <si>
+    <t>house/house089.png</t>
+  </si>
+  <si>
+    <t>house/house077.png</t>
+  </si>
+  <si>
+    <t>face/face077.png</t>
+  </si>
+  <si>
     <t>face/face097.png</t>
   </si>
   <si>
-    <t>car/car113.png</t>
-  </si>
-  <si>
-    <t>face/face096.png</t>
-  </si>
-  <si>
-    <t>face/face073.png</t>
-  </si>
-  <si>
-    <t>face/face072.png</t>
-  </si>
-  <si>
-    <t>car/car109.png</t>
-  </si>
-  <si>
-    <t>face/face091.png</t>
-  </si>
-  <si>
-    <t>car/car066.png</t>
-  </si>
-  <si>
-    <t>car/car067.png</t>
-  </si>
-  <si>
-    <t>car/car121.png</t>
-  </si>
-  <si>
-    <t>car/car081.png</t>
-  </si>
-  <si>
-    <t>car/car082.png</t>
-  </si>
-  <si>
-    <t>face/face108.png</t>
-  </si>
-  <si>
-    <t>car/car102.png</t>
-  </si>
-  <si>
-    <t>face/face090.png</t>
-  </si>
-  <si>
-    <t>face/face080.png</t>
-  </si>
-  <si>
-    <t>face/face071.png</t>
-  </si>
-  <si>
-    <t>car/car071.png</t>
-  </si>
-  <si>
-    <t>car/car080.png</t>
-  </si>
-  <si>
-    <t>car/car089.png</t>
-  </si>
-  <si>
-    <t>face/face065.png</t>
-  </si>
-  <si>
-    <t>face/face092.png</t>
-  </si>
-  <si>
-    <t>face/face121.png</t>
-  </si>
-  <si>
-    <t>face/face103.png</t>
-  </si>
-  <si>
-    <t>face/face085.png</t>
-  </si>
-  <si>
-    <t>car/car111.png</t>
-  </si>
-  <si>
-    <t>car/car112.png</t>
-  </si>
-  <si>
-    <t>car/car069.png</t>
-  </si>
-  <si>
-    <t>car/car116.png</t>
-  </si>
-  <si>
-    <t>face/face086.png</t>
-  </si>
-  <si>
-    <t>car/car077.png</t>
-  </si>
-  <si>
-    <t>face/face123.png</t>
+    <t>face/face100.png</t>
+  </si>
+  <si>
+    <t>house/house069.png</t>
+  </si>
+  <si>
+    <t>face/face067.png</t>
+  </si>
+  <si>
+    <t>face/face083.png</t>
+  </si>
+  <si>
+    <t>house/house115.png</t>
+  </si>
+  <si>
+    <t>face/face088.png</t>
+  </si>
+  <si>
+    <t>house/house087.png</t>
+  </si>
+  <si>
+    <t>house/house107.png</t>
+  </si>
+  <si>
+    <t>house/house080.png</t>
+  </si>
+  <si>
+    <t>house/house105.png</t>
+  </si>
+  <si>
+    <t>quellen</t>
+  </si>
+  <si>
+    <t>hören</t>
+  </si>
+  <si>
+    <t>proben</t>
+  </si>
+  <si>
+    <t>ändern</t>
+  </si>
+  <si>
+    <t>süßen</t>
+  </si>
+  <si>
+    <t>danken</t>
+  </si>
+  <si>
+    <t>münzen</t>
+  </si>
+  <si>
+    <t>legen</t>
+  </si>
+  <si>
+    <t>binden</t>
+  </si>
+  <si>
+    <t>lächeln</t>
+  </si>
+  <si>
+    <t>duschen</t>
+  </si>
+  <si>
+    <t>achten</t>
+  </si>
+  <si>
+    <t>zielen</t>
+  </si>
+  <si>
+    <t>streifen</t>
+  </si>
+  <si>
+    <t>rechnen</t>
+  </si>
+  <si>
+    <t>wehen</t>
+  </si>
+  <si>
+    <t>passen</t>
+  </si>
+  <si>
+    <t>reisen</t>
+  </si>
+  <si>
+    <t>lernen</t>
+  </si>
+  <si>
+    <t>wachsen</t>
+  </si>
+  <si>
+    <t>stoppen</t>
+  </si>
+  <si>
+    <t>planen</t>
+  </si>
+  <si>
+    <t>bergen</t>
+  </si>
+  <si>
+    <t>wecken</t>
   </si>
   <si>
     <t>atmen</t>
   </si>
   <si>
-    <t>nullen</t>
-  </si>
-  <si>
-    <t>deuten</t>
-  </si>
-  <si>
-    <t>süßen</t>
-  </si>
-  <si>
-    <t>reisen</t>
-  </si>
-  <si>
-    <t>sparen</t>
-  </si>
-  <si>
-    <t>hacken</t>
-  </si>
-  <si>
-    <t>legen</t>
-  </si>
-  <si>
-    <t>wehen</t>
-  </si>
-  <si>
-    <t>frischen</t>
-  </si>
-  <si>
-    <t>danken</t>
-  </si>
-  <si>
-    <t>passen</t>
-  </si>
-  <si>
-    <t>küssen</t>
-  </si>
-  <si>
-    <t>meinen</t>
-  </si>
-  <si>
-    <t>ändern</t>
+    <t>spüren</t>
+  </si>
+  <si>
+    <t>grenzen</t>
   </si>
   <si>
     <t>öffnen</t>
   </si>
   <si>
-    <t>wählen</t>
-  </si>
-  <si>
-    <t>wecken</t>
-  </si>
-  <si>
-    <t>leeren</t>
-  </si>
-  <si>
-    <t>tollen</t>
-  </si>
-  <si>
-    <t>rechnen</t>
-  </si>
-  <si>
-    <t>zögern</t>
-  </si>
-  <si>
-    <t>bergen</t>
-  </si>
-  <si>
-    <t>dienen</t>
-  </si>
-  <si>
-    <t>planen</t>
-  </si>
-  <si>
     <t>herrschen</t>
   </si>
   <si>
+    <t>angeln</t>
+  </si>
+  <si>
+    <t>prüfen</t>
+  </si>
+  <si>
     <t>stoßen</t>
   </si>
   <si>
-    <t>piepen</t>
-  </si>
-  <si>
-    <t>hassen</t>
-  </si>
-  <si>
-    <t>duschen</t>
-  </si>
-  <si>
-    <t>fließen</t>
-  </si>
-  <si>
-    <t>streifen</t>
-  </si>
-  <si>
     <t>face</t>
   </si>
   <si>
-    <t>car</t>
+    <t>house</t>
   </si>
 </sst>
 </file>
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -718,7 +718,7 @@
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -746,7 +746,7 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -788,7 +788,7 @@
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -816,7 +816,7 @@
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -830,7 +830,7 @@
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -844,7 +844,7 @@
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -928,7 +928,7 @@
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -956,7 +956,7 @@
         <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -984,7 +984,7 @@
         <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1012,7 +1012,7 @@
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1040,7 +1040,7 @@
         <v>66</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add working set of sequences
</commit_message>
<xml_diff>
--- a/sequences/00_cues.xlsx
+++ b/sequences/00_cues.xlsx
@@ -25,202 +25,202 @@
     <t>category</t>
   </si>
   <si>
-    <t>face/face070.png</t>
-  </si>
-  <si>
-    <t>house/house095.png</t>
-  </si>
-  <si>
-    <t>house/house075.png</t>
-  </si>
-  <si>
-    <t>face/face069.png</t>
-  </si>
-  <si>
-    <t>face/face108.png</t>
-  </si>
-  <si>
-    <t>house/house125.png</t>
-  </si>
-  <si>
-    <t>face/face092.png</t>
-  </si>
-  <si>
-    <t>house/house117.png</t>
-  </si>
-  <si>
-    <t>face/face099.png</t>
-  </si>
-  <si>
-    <t>house/house091.png</t>
-  </si>
-  <si>
-    <t>face/face094.png</t>
-  </si>
-  <si>
-    <t>house/house094.png</t>
-  </si>
-  <si>
-    <t>face/face064.png</t>
-  </si>
-  <si>
-    <t>face/face096.png</t>
-  </si>
-  <si>
-    <t>face/face101.png</t>
-  </si>
-  <si>
-    <t>house/house082.png</t>
-  </si>
-  <si>
-    <t>house/house086.png</t>
-  </si>
-  <si>
-    <t>face/face090.png</t>
-  </si>
-  <si>
-    <t>house/house089.png</t>
-  </si>
-  <si>
-    <t>house/house077.png</t>
-  </si>
-  <si>
-    <t>face/face077.png</t>
-  </si>
-  <si>
-    <t>face/face097.png</t>
-  </si>
-  <si>
-    <t>face/face100.png</t>
-  </si>
-  <si>
-    <t>house/house069.png</t>
-  </si>
-  <si>
-    <t>face/face067.png</t>
-  </si>
-  <si>
-    <t>face/face083.png</t>
-  </si>
-  <si>
-    <t>house/house115.png</t>
-  </si>
-  <si>
-    <t>face/face088.png</t>
-  </si>
-  <si>
-    <t>house/house087.png</t>
-  </si>
-  <si>
-    <t>house/house107.png</t>
-  </si>
-  <si>
-    <t>house/house080.png</t>
-  </si>
-  <si>
-    <t>house/house105.png</t>
-  </si>
-  <si>
-    <t>quellen</t>
+    <t>house/house023.jpg</t>
+  </si>
+  <si>
+    <t>house/house003.jpg</t>
+  </si>
+  <si>
+    <t>face/face021.jpg</t>
+  </si>
+  <si>
+    <t>house/house002.jpg</t>
+  </si>
+  <si>
+    <t>house/house006.jpg</t>
+  </si>
+  <si>
+    <t>house/house011.jpg</t>
+  </si>
+  <si>
+    <t>face/face008.jpg</t>
+  </si>
+  <si>
+    <t>face/face013.jpg</t>
+  </si>
+  <si>
+    <t>face/face004.jpg</t>
+  </si>
+  <si>
+    <t>face/face014.jpg</t>
+  </si>
+  <si>
+    <t>face/face019.jpg</t>
+  </si>
+  <si>
+    <t>house/house004.jpg</t>
+  </si>
+  <si>
+    <t>house/house028.jpg</t>
+  </si>
+  <si>
+    <t>house/house020.jpg</t>
+  </si>
+  <si>
+    <t>face/face005.jpg</t>
+  </si>
+  <si>
+    <t>house/house021.jpg</t>
+  </si>
+  <si>
+    <t>house/house009.jpg</t>
+  </si>
+  <si>
+    <t>house/house015.jpg</t>
+  </si>
+  <si>
+    <t>face/face027.jpg</t>
+  </si>
+  <si>
+    <t>face/face016.jpg</t>
+  </si>
+  <si>
+    <t>face/face015.jpg</t>
+  </si>
+  <si>
+    <t>house/house001.jpg</t>
+  </si>
+  <si>
+    <t>house/house008.jpg</t>
+  </si>
+  <si>
+    <t>house/house012.jpg</t>
+  </si>
+  <si>
+    <t>face/face022.jpg</t>
+  </si>
+  <si>
+    <t>face/face010.jpg</t>
+  </si>
+  <si>
+    <t>house/house005.jpg</t>
+  </si>
+  <si>
+    <t>face/face024.jpg</t>
+  </si>
+  <si>
+    <t>face/face011.jpg</t>
+  </si>
+  <si>
+    <t>house/house014.jpg</t>
+  </si>
+  <si>
+    <t>face/face028.jpg</t>
+  </si>
+  <si>
+    <t>face/face012.jpg</t>
+  </si>
+  <si>
+    <t>herrschen</t>
+  </si>
+  <si>
+    <t>betteln</t>
+  </si>
+  <si>
+    <t>heißen</t>
+  </si>
+  <si>
+    <t>nullen</t>
   </si>
   <si>
     <t>hören</t>
   </si>
   <si>
-    <t>proben</t>
-  </si>
-  <si>
-    <t>ändern</t>
-  </si>
-  <si>
-    <t>süßen</t>
-  </si>
-  <si>
-    <t>danken</t>
-  </si>
-  <si>
-    <t>münzen</t>
-  </si>
-  <si>
-    <t>legen</t>
+    <t>piepen</t>
+  </si>
+  <si>
+    <t>lassen</t>
   </si>
   <si>
     <t>binden</t>
   </si>
   <si>
+    <t>planen</t>
+  </si>
+  <si>
+    <t>öffnen</t>
+  </si>
+  <si>
+    <t>reisen</t>
+  </si>
+  <si>
+    <t>kranken</t>
+  </si>
+  <si>
     <t>lächeln</t>
   </si>
   <si>
+    <t>grenzen</t>
+  </si>
+  <si>
+    <t>holen</t>
+  </si>
+  <si>
+    <t>rufen</t>
+  </si>
+  <si>
+    <t>passen</t>
+  </si>
+  <si>
+    <t>frischen</t>
+  </si>
+  <si>
+    <t>wählen</t>
+  </si>
+  <si>
+    <t>dienen</t>
+  </si>
+  <si>
+    <t>hacken</t>
+  </si>
+  <si>
+    <t>wachsen</t>
+  </si>
+  <si>
+    <t>wecken</t>
+  </si>
+  <si>
+    <t>meinen</t>
+  </si>
+  <si>
+    <t>bauen</t>
+  </si>
+  <si>
+    <t>zögern</t>
+  </si>
+  <si>
+    <t>stoßen</t>
+  </si>
+  <si>
+    <t>atmen</t>
+  </si>
+  <si>
+    <t>narren</t>
+  </si>
+  <si>
+    <t>mögen</t>
+  </si>
+  <si>
     <t>duschen</t>
   </si>
   <si>
-    <t>achten</t>
-  </si>
-  <si>
-    <t>zielen</t>
-  </si>
-  <si>
-    <t>streifen</t>
-  </si>
-  <si>
-    <t>rechnen</t>
-  </si>
-  <si>
-    <t>wehen</t>
-  </si>
-  <si>
-    <t>passen</t>
-  </si>
-  <si>
-    <t>reisen</t>
-  </si>
-  <si>
-    <t>lernen</t>
-  </si>
-  <si>
-    <t>wachsen</t>
-  </si>
-  <si>
-    <t>stoppen</t>
-  </si>
-  <si>
-    <t>planen</t>
-  </si>
-  <si>
-    <t>bergen</t>
-  </si>
-  <si>
-    <t>wecken</t>
-  </si>
-  <si>
-    <t>atmen</t>
-  </si>
-  <si>
-    <t>spüren</t>
-  </si>
-  <si>
-    <t>grenzen</t>
-  </si>
-  <si>
-    <t>öffnen</t>
-  </si>
-  <si>
-    <t>herrschen</t>
-  </si>
-  <si>
-    <t>angeln</t>
-  </si>
-  <si>
-    <t>prüfen</t>
-  </si>
-  <si>
-    <t>stoßen</t>
+    <t>kriegen</t>
+  </si>
+  <si>
+    <t>house</t>
   </si>
   <si>
     <t>face</t>
-  </si>
-  <si>
-    <t>house</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -676,7 +676,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -690,7 +690,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -718,7 +718,7 @@
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -746,7 +746,7 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -760,7 +760,7 @@
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -802,7 +802,7 @@
         <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -816,7 +816,7 @@
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -830,7 +830,7 @@
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -886,7 +886,7 @@
         <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -928,7 +928,7 @@
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -942,7 +942,7 @@
         <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -956,7 +956,7 @@
         <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -970,7 +970,7 @@
         <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -984,7 +984,7 @@
         <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1012,7 +1012,7 @@
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4">

</xml_diff>